<commit_message>
Update the Sprint Sheet
</commit_message>
<xml_diff>
--- a/documentation/Sprint Sheet Two0owT.xlsx
+++ b/documentation/Sprint Sheet Two0owT.xlsx
@@ -1073,11 +1073,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="69855389"/>
-        <c:axId val="600123346"/>
+        <c:axId val="1547725831"/>
+        <c:axId val="951797288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69855389"/>
+        <c:axId val="1547725831"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1129,10 +1129,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600123346"/>
+        <c:crossAx val="951797288"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="600123346"/>
+        <c:axId val="951797288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1196,7 +1196,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69855389"/>
+        <c:crossAx val="1547725831"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1325,11 +1325,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1788534083"/>
-        <c:axId val="684961323"/>
+        <c:axId val="929038257"/>
+        <c:axId val="527994467"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1788534083"/>
+        <c:axId val="929038257"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,10 +1381,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="684961323"/>
+        <c:crossAx val="527994467"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="684961323"/>
+        <c:axId val="527994467"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1448,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1788534083"/>
+        <c:crossAx val="929038257"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1566,11 +1566,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="776639328"/>
-        <c:axId val="855261648"/>
+        <c:axId val="938147110"/>
+        <c:axId val="14675029"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="776639328"/>
+        <c:axId val="938147110"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1622,10 +1622,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="855261648"/>
+        <c:crossAx val="14675029"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="855261648"/>
+        <c:axId val="14675029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1689,7 +1689,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="776639328"/>
+        <c:crossAx val="938147110"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1818,11 +1818,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1273021984"/>
-        <c:axId val="1203832193"/>
+        <c:axId val="961029084"/>
+        <c:axId val="387749000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1273021984"/>
+        <c:axId val="961029084"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1874,10 +1874,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1203832193"/>
+        <c:crossAx val="387749000"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1203832193"/>
+        <c:axId val="387749000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1941,7 +1941,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1273021984"/>
+        <c:crossAx val="961029084"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2058,11 +2058,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1435028104"/>
-        <c:axId val="2023751196"/>
+        <c:axId val="1490980766"/>
+        <c:axId val="709337301"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1435028104"/>
+        <c:axId val="1490980766"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2114,10 +2114,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2023751196"/>
+        <c:crossAx val="709337301"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2023751196"/>
+        <c:axId val="709337301"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,7 +2181,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1435028104"/>
+        <c:crossAx val="1490980766"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>